<commit_message>
Aktualizacja algorytmow i dodanie testow
</commit_message>
<xml_diff>
--- a/tests/output/Algorytm Roju cząstek/pso_memory_results.xlsx
+++ b/tests/output/Algorytm Roju cząstek/pso_memory_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,63 +436,59 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Instancja problemu</t>
+          <t>Plik</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Średnie zużycie pamięci (MB)</t>
+          <t>Parametry</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Parametry</t>
+          <t>Aktualne użycie pamięci</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Szczytowe użycie pamięci</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>data/280_1.txt</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0.376896</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Cząstki: 10, Iteracje: 50</t>
-        </is>
+          <t>data/50_1.txt</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>dobre</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.3469924926757812</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.355438232421875</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>data/2000_1.txt</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>5.080224</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Cząstki: 10, Iteracje: 50</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>data/4461_1.txt</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>11.433368</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Cząstki: 10, Iteracje: 50</t>
-        </is>
+          <t>data/50_1.txt</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>słabe</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.06217193603515625</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0703277587890625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>